<commit_message>
Updated who has which devices in the Orders spreadsheet
</commit_message>
<xml_diff>
--- a/UVM-NRT-RoS/equipment-records/Orders.xlsx
+++ b/UVM-NRT-RoS/equipment-records/Orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f59c65449ee1dfc/Documents/UVM/2023-2024/CIROH Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{A247FFB5-95D5-4EBF-AF1B-C6DB9864D309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{819A2220-5A27-4EC6-93C2-D6CDA21234D3}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{A247FFB5-95D5-4EBF-AF1B-C6DB9864D309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC9D64A5-B316-46D8-99DB-2B31E699DC47}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CE922E94-D1B5-48D4-B95E-289D5B1A9D60}"/>
+    <workbookView xWindow="264" yWindow="1128" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{CE922E94-D1B5-48D4-B95E-289D5B1A9D60}"/>
   </bookViews>
   <sheets>
     <sheet name="Order 9-20-23" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>Item</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Rachael (1), Quimby (2), Spencer (1)</t>
+  </si>
+  <si>
+    <t>Delivered 10/5/23</t>
+  </si>
+  <si>
+    <t>Yes!</t>
+  </si>
+  <si>
+    <t>Lars</t>
   </si>
 </sst>
 </file>
@@ -574,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0169E8-44C1-4515-8783-23B235C606F5}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D5D17-2D4C-4E1D-9379-F50B81DC45FA}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,6 +1048,15 @@
       <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="4"/>

</xml_diff>